<commit_message>
change Functions_LMS.xlsx and Review1_v1.0.1.docx
</commit_message>
<xml_diff>
--- a/Document/Functions_LMS.xlsx
+++ b/Document/Functions_LMS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="111">
   <si>
     <t>Table</t>
   </si>
@@ -276,6 +276,80 @@
   </si>
   <si>
     <t>OrderDetail_Update</t>
+  </si>
+  <si>
+    <t>Delete Order</t>
+  </si>
+  <si>
+    <t>Orders_Delete</t>
+  </si>
+  <si>
+    <t>Order_Id</t>
+  </si>
+  <si>
+    <t>Delete OrderDetail</t>
+  </si>
+  <si>
+    <t>OrderDetail_Delete</t>
+  </si>
+  <si>
+    <t>Store Reference</t>
+  </si>
+  <si>
+    <t>Book_ISBN,Copy_Id(if)</t>
+  </si>
+  <si>
+    <t>action delete is update field isDeleted = 1
+check Cop_Status = 1 thì mới có thể Delete</t>
+  </si>
+  <si>
+    <t>đối với kiễu chuỗi defaul value  = '' or value = null
+đối với kiểu số default value = null or value = -1
+đối với kiểu ngày tháng thành truyền vào là chuỗi và nhận là chuỗi - làm điều kiện search sẽ dễ hơn</t>
+  </si>
+  <si>
+    <t>Order_Id(if), Mem_Id(if), Order_CreateDate(if),Order_DueDate(if)</t>
+  </si>
+  <si>
+    <t>action delete is update field isDeleted = 1
+Check count(OrderDetail) by ISBN If  = 0 then Call Delete Order</t>
+  </si>
+  <si>
+    <t>Fines</t>
+  </si>
+  <si>
+    <t>Insert Fine</t>
+  </si>
+  <si>
+    <t>Update Fine</t>
+  </si>
+  <si>
+    <t>Paid Fine</t>
+  </si>
+  <si>
+    <t>action delete is update field isDeleted = 1
+Check count(OrderDetail_Status =0) by ISBN if = 0 Call OrderDetail_Delete (cancel all detail). If not cancel action</t>
+  </si>
+  <si>
+    <t>Call OrderDetails_Insert</t>
+  </si>
+  <si>
+    <t>Order_Id,Mem_Id,Order_DueDate</t>
+  </si>
+  <si>
+    <t>Delete member</t>
+  </si>
+  <si>
+    <t>Delete Staff</t>
+  </si>
+  <si>
+    <t>Members_Delete</t>
+  </si>
+  <si>
+    <t>action delete is update field isDeleted = 1</t>
+  </si>
+  <si>
+    <t>Staffs_Delete</t>
   </si>
   <si>
     <r>
@@ -295,67 +369,8 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">
-Amount is number of book will be loop.it will call function returnMaxId. After that Book_Id generated = Book_ISBN + (max number  + (3 letter number  + 1)) (append String)</t>
+</t>
     </r>
-  </si>
-  <si>
-    <t>Delete Order</t>
-  </si>
-  <si>
-    <t>Orders_Delete</t>
-  </si>
-  <si>
-    <t>Order_Id</t>
-  </si>
-  <si>
-    <t>Delete OrderDetail</t>
-  </si>
-  <si>
-    <t>OrderDetail_Delete</t>
-  </si>
-  <si>
-    <t>Store Reference</t>
-  </si>
-  <si>
-    <t>Book_ISBN,Copy_Id(if)</t>
-  </si>
-  <si>
-    <t>action delete is update field isDeleted = 1
-check Cop_Status = 1 thì mới có thể Delete</t>
-  </si>
-  <si>
-    <t>đối với kiễu chuỗi defaul value  = '' or value = null
-đối với kiểu số default value = null or value = -1
-đối với kiểu ngày tháng thành truyền vào là chuỗi và nhận là chuỗi - làm điều kiện search sẽ dễ hơn</t>
-  </si>
-  <si>
-    <t>Order_Id(if), Mem_Id(if), Order_CreateDate(if),Order_DueDate(if)</t>
-  </si>
-  <si>
-    <t>action delete is update field isDeleted = 1
-Check count(OrderDetail) by ISBN If  = 0 then Call Delete Order</t>
-  </si>
-  <si>
-    <t>Fines</t>
-  </si>
-  <si>
-    <t>Insert Fine</t>
-  </si>
-  <si>
-    <t>Update Fine</t>
-  </si>
-  <si>
-    <t>Paid Fine</t>
-  </si>
-  <si>
-    <t>action delete is update field isDeleted = 1
-Check count(OrderDetail_Status =0) by ISBN if = 0 Call OrderDetail_Delete (cancel all detail). If not cancel action</t>
-  </si>
-  <si>
-    <t>Call OrderDetails_Insert</t>
-  </si>
-  <si>
-    <t>Order_Id,Mem_Id,Order_DueDate</t>
   </si>
 </sst>
 </file>
@@ -390,12 +405,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -425,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -441,6 +462,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -765,7 +789,7 @@
     <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -776,7 +800,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
@@ -788,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
@@ -802,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
@@ -816,380 +840,422 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="6" t="s">
+      <c r="G6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="6" t="s">
+      <c r="G7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
+      <c r="G12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
+      <c r="G13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+    <row r="16" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D16" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+      <c r="G16" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D17" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>59</v>
+      <c r="G17" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="6" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+    <row r="22" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C21" s="6" t="s">
+      <c r="G22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="G23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="6" t="s">
+      <c r="F26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="C28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="C26" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="C29" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H29" s="7" t="s">
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="6" t="s">
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="6" t="s">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1244,7 +1310,7 @@
         <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Functions_LMS.xlsx - Add Store getCategoryListWithBookNumber Categories - Start loading - DONE UyTPV_SQLWorking.sql - Insert Categories, Insert Book demo data - Create Store getCategoryListWithBookNumber
</commit_message>
<xml_diff>
--- a/Document/Functions_LMS.xlsx
+++ b/Document/Functions_LMS.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
   <si>
     <t>Table</t>
   </si>
@@ -683,6 +683,12 @@
   </si>
   <si>
     <t>no need</t>
+  </si>
+  <si>
+    <t>getCategoryListWithBookNumber</t>
+  </si>
+  <si>
+    <t>Get Category List With Book Number</t>
   </si>
 </sst>
 </file>
@@ -802,10 +808,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -874,7 +880,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -909,7 +915,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1118,17 +1124,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="60" style="7" customWidth="1"/>
@@ -1161,10 +1170,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1183,8 +1192,8 @@
       <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
@@ -1201,8 +1210,8 @@
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="13" t="s">
         <v>73</v>
       </c>
@@ -1221,8 +1230,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="13" t="s">
         <v>22</v>
       </c>
@@ -1353,10 +1362,10 @@
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="17">
         <v>3</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -1375,8 +1384,8 @@
       <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
@@ -1393,8 +1402,8 @@
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="13" t="s">
         <v>77</v>
       </c>
@@ -1413,393 +1422,409 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="13" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="F15" s="14"/>
       <c r="G15" s="13" t="s">
         <v>0</v>
       </c>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+    <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
         <v>4</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B17" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="G17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="19"/>
       <c r="C18" s="10" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>81</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E18" s="10"/>
       <c r="F18" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="19"/>
       <c r="C19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11" t="s">
+      <c r="E20" s="10"/>
+      <c r="F20" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
         <v>5</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D21" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>83</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="17"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="14" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="16" t="s">
-        <v>119</v>
+      <c r="H22" s="14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="13" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
-        <v>6</v>
-      </c>
-      <c r="B24" s="19" t="s">
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>6</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="11" t="s">
+      <c r="G25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="10" t="s">
+    <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11" t="s">
+      <c r="E26" s="10"/>
+      <c r="F26" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G26" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
         <v>7</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C27" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D27" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14" t="s">
+      <c r="E27" s="13"/>
+      <c r="F27" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="14"/>
-    </row>
-    <row r="27" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="13" t="s">
+      <c r="G27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F28" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="14" t="s">
+      <c r="G28" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="13" t="s">
+    <row r="29" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D29" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="14"/>
-    </row>
-    <row r="29" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="14" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="20">
         <v>8</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B31" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="11" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H31" s="11"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="19"/>
       <c r="C32" s="10" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G33" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H32" s="11"/>
+      <c r="H33" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1946,7 +1971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update some store by trunghth
</commit_message>
<xml_diff>
--- a/Document/Functions_LMS.xlsx
+++ b/Document/Functions_LMS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="148">
   <si>
     <t>Table</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Staff_Id</t>
   </si>
   <si>
-    <t>Get member by parameters</t>
-  </si>
-  <si>
     <t>Get Staff by parameters</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
   </si>
   <si>
     <t>Insert Staff</t>
-  </si>
-  <si>
-    <t>Mem_Id(if),Mem_Email(if),Mem_Firstname(if)</t>
   </si>
   <si>
     <t>Staff_Id(if),Staff_Email(if),Staff_Firstname(if),Staff_Login(if)</t>
@@ -689,6 +683,42 @@
   </si>
   <si>
     <t>Get Category List With Book Number</t>
+  </si>
+  <si>
+    <t>Get member by parameters (trunghth)</t>
+  </si>
+  <si>
+    <t>Members_GetIRCountInformation</t>
+  </si>
+  <si>
+    <t>Mem_No</t>
+  </si>
+  <si>
+    <t>Mem_No(if),Mem_name(if),Mem_Email(if),Mem_Phone(if)</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Books_getListBookByFilter</t>
+  </si>
+  <si>
+    <t>Get Book by parameters Filter Issue Form (trunghth)</t>
+  </si>
+  <si>
+    <t>Get Count Issued Book By Member (trunghth)</t>
+  </si>
+  <si>
+    <t>Book_ISBN(if),Book_Title(if),Cat_Id(if)</t>
+  </si>
+  <si>
+    <t>Copies_getLastestIsFree</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Get Copy for issuing which is free-random (trunghth)</t>
   </si>
 </sst>
 </file>
@@ -764,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -814,10 +844,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -880,7 +943,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -915,7 +978,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1124,20 +1187,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="38.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="60" style="7" customWidth="1"/>
@@ -1157,7 +1220,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>1</v>
@@ -1170,10 +1233,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1184,7 +1247,7 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>6</v>
@@ -1192,8 +1255,8 @@
       <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
@@ -1202,7 +1265,7 @@
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>6</v>
@@ -1210,13 +1273,13 @@
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14" t="s">
@@ -1226,175 +1289,175 @@
         <v>6</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="19"/>
       <c r="C7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="19"/>
+    <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="10" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>109</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="11" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="10" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="G11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
         <v>3</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
+      <c r="B13" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>6</v>
@@ -1402,429 +1465,483 @@
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="13" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="14" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>109</v>
-      </c>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="13" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="G15" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="13" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="F16" s="14"/>
       <c r="G16" s="13" t="s">
         <v>0</v>
       </c>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+    <row r="17" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22">
         <v>4</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="19"/>
+      <c r="B18" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="C18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="F18" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="19"/>
+      <c r="H18" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="F20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="10" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:8" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <v>5</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
-        <v>5</v>
-      </c>
-      <c r="B21" s="18" t="s">
+      <c r="D23" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="14" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
+      <c r="H23" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="13" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="14" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
         <v>6</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G25" s="10" t="s">
+      <c r="H24" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H25" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="19"/>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="23"/>
+      <c r="F27" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A28" s="22">
+        <v>6</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E29" s="10"/>
+      <c r="F29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20">
+        <v>7</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11" t="s">
+      <c r="C30" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
-        <v>7</v>
-      </c>
-      <c r="B27" s="18" t="s">
+      <c r="D30" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="14"/>
-    </row>
-    <row r="28" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="14" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
-        <v>8</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="19"/>
-      <c r="C32" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C32" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
       <c r="B33" s="19"/>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="22">
+        <v>8</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="10" t="s">
+    </row>
+    <row r="36" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" s="10" t="s">
+      <c r="G36" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="11"/>
+      <c r="H36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A28:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1849,15 +1966,15 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1865,47 +1982,47 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1937,7 +2054,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1953,13 +2070,13 @@
     </row>
     <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1982,26 +2099,26 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
         <v>133</v>
-      </c>
-      <c r="C4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Book get by ISBN
</commit_message>
<xml_diff>
--- a/Document/Functions_LMS.xlsx
+++ b/Document/Functions_LMS.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="150">
   <si>
     <t>Table</t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>Get Copy for issuing which is free-random (trunghth)</t>
+  </si>
+  <si>
+    <t>Books_getByISBN</t>
+  </si>
+  <si>
+    <t>Get Book By ISBN use view table (trunghth)</t>
   </si>
 </sst>
 </file>
@@ -844,43 +850,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1187,13 +1193,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1233,10 +1239,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1255,8 +1261,8 @@
       <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
@@ -1273,8 +1279,8 @@
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="13" t="s">
         <v>71</v>
       </c>
@@ -1292,47 +1298,47 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23" t="s">
+    <row r="5" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="19" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="19" t="s">
         <v>140</v>
       </c>
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="31">
         <v>2</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1351,8 +1357,8 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="10" t="s">
         <v>23</v>
       </c>
@@ -1369,8 +1375,8 @@
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
@@ -1387,8 +1393,8 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="10" t="s">
         <v>73</v>
       </c>
@@ -1407,8 +1413,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1425,8 +1431,8 @@
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="10" t="s">
         <v>62</v>
       </c>
@@ -1443,10 +1449,10 @@
       <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+      <c r="A13" s="28">
         <v>3</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -1465,8 +1471,8 @@
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="13" t="s">
         <v>28</v>
       </c>
@@ -1483,8 +1489,8 @@
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="13" t="s">
         <v>75</v>
       </c>
@@ -1503,8 +1509,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="13" t="s">
         <v>135</v>
       </c>
@@ -1519,8 +1525,8 @@
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="13" t="s">
         <v>29</v>
       </c>
@@ -1537,10 +1543,10 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+      <c r="A18" s="31">
         <v>4</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="30" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1563,8 +1569,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="10" t="s">
         <v>42</v>
       </c>
@@ -1581,8 +1587,8 @@
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="10" t="s">
         <v>77</v>
       </c>
@@ -1603,8 +1609,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="21"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="10" t="s">
         <v>43</v>
       </c>
@@ -1620,328 +1626,346 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27" t="s">
+    <row r="22" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D23" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28" t="s">
+      <c r="E23" s="23"/>
+      <c r="F23" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G23" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="28"/>
-    </row>
-    <row r="23" spans="1:8" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="H23" s="24"/>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
         <v>5</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B24" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D24" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="19"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="14" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="16" t="s">
-        <v>117</v>
+      <c r="H25" s="14" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="13" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G27" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="14"/>
-    </row>
-    <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="23" t="s">
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D28" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="16" t="s">
+      <c r="E28" s="19"/>
+      <c r="F28" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G28" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
         <v>6</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B29" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G29" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H29" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="10" t="s">
+    <row r="30" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11" t="s">
+      <c r="E30" s="10"/>
+      <c r="F30" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28">
         <v>7</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B31" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="14" t="s">
+      <c r="E31" s="13"/>
+      <c r="F31" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>122</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="13" t="s">
+    <row r="33" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D33" s="13" t="s">
         <v>94</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" spans="1:8" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="14" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="14"/>
+    </row>
+    <row r="34" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="22">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
         <v>8</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B35" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C35" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>99</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="11" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="21"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="10" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G37" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H36" s="11"/>
+      <c r="H37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A28:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>